<commit_message>
can import system fields
</commit_message>
<xml_diff>
--- a/src/test/resources/dataimports-test.xlsx
+++ b/src/test/resources/dataimports-test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C7A31C-F31B-C84A-8125-B875055A52B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>NUMBER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -209,14 +210,34 @@
   </si>
   <si>
     <t>无效日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属用户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rebuild</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOUSER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user@email.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,7 +308,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -362,6 +383,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -397,6 +435,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,21 +627,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="5" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -635,8 +690,11 @@
       <c r="P1" t="s">
         <v>33</v>
       </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -685,8 +743,11 @@
       <c r="P2" t="s">
         <v>39</v>
       </c>
+      <c r="Q2" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -729,8 +790,11 @@
       <c r="P3" t="s">
         <v>40</v>
       </c>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -773,8 +837,11 @@
       <c r="P4" t="s">
         <v>40</v>
       </c>
+      <c r="Q4" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -810,19 +877,23 @@
       </c>
       <c r="P5" t="s">
         <v>38</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
-    <hyperlink ref="I4" r:id="rId5"/>
-    <hyperlink ref="I5" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="Q5" r:id="rId7" xr:uid="{DA069E45-D224-3B4D-9FC8-8D22E8191F31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="257" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="257" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>